<commit_message>
First Alt captured. Now figure it out
</commit_message>
<xml_diff>
--- a/CH-77 Character-Based Rhombus.xlsx
+++ b/CH-77 Character-Based Rhombus.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463F93CC-2493-4361-99F8-5C93D0B809EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B47563-482B-4243-8531-2E003142DFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="rhombus">_xlfn.LAMBDA(_xlpm.n,     _xlfn.LET(         _xlpm.m, INT(_xlpm.n / 2),         _xlpm.f, _xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlop.x,_xlop.y, ABS(_xlpm.m - _xlpm.x - _xlpm.r + 1) + ABS(_xlpm.m - _xlpm.y - _xlpm.c + 1)),         _xlpm.ff, _xlfn.LAMBDA(_xlpm.r,_xlpm.c,             IF(                 IF(ISODD(_xlpm.n), _xlpm.f(_xlpm.r, _xlpm.c) &lt;= _xlpm.m, OR(_xlpm.f(_xlpm.r, _xlpm.c, 1, 1) &lt; _xlpm.m, _xlpm.f(_xlpm.r, _xlpm.c, , 1) &lt; _xlpm.m, _xlpm.f(_xlpm.r, _xlpm.c, 1) &lt; _xlpm.m, _xlpm.f(_xlpm.r, _xlpm.c) &lt; _xlpm.m)),                 "*",                 ""             )         ),         _xlfn.MAKEARRAY(_xlpm.n, _xlpm.n, _xlpm.ff)     ) )</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="1">
   <si>
     <t>*</t>
   </si>
@@ -94,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -106,6 +133,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -275,6 +305,72 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>138430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>111760</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>2540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F05BBE3-2E6E-25B2-481E-389AB4442E27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="10552430"/>
+          <a:ext cx="8893810" cy="5204460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -534,11 +630,38 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="1547" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{BC71E309-4000-4F90-8125-FCF586DFFCC7}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
@@ -991,4 +1114,1540 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B17870-5941-4C59-8CD8-DDAC51A6FF70}">
+  <dimension ref="C1:Q25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.77734375" customWidth="1"/>
+    <col min="3" max="4" width="2.44140625" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" style="4" customWidth="1"/>
+    <col min="6" max="17" width="2.44140625" customWidth="1"/>
+    <col min="18" max="19" width="2.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:17" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="4"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="4"/>
+      <c r="F5"/>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="4"/>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36980439-0376-4A92-93D2-9D66C85EB6B6}">
+  <dimension ref="C1:BD61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="AG37" sqref="AG37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="2.77734375" customWidth="1"/>
+    <col min="3" max="4" width="2.44140625" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" style="4" customWidth="1"/>
+    <col min="6" max="17" width="2.44140625" customWidth="1"/>
+    <col min="18" max="19" width="2.77734375" customWidth="1"/>
+    <col min="21" max="32" width="2.44140625" customWidth="1"/>
+    <col min="36" max="56" width="2.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:48" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="3:48" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:48" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="4"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:48" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV4"/>
+    </row>
+    <row r="5" spans="3:48" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="4"/>
+      <c r="F5"/>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:48" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="4"/>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:48" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="3:48" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="3"/>
+    </row>
+    <row r="35" spans="47:56" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AU35" s="6" t="str" cm="1">
+        <f t="array" ref="AU35:BD44">_xlfn.LAMBDA(_xlpm.n,
+    _xlfn.LET(
+        _xlpm.m, INT(_xlpm.n / 2),
+        _xlpm.f, _xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlop.x,_xlop.y, ABS(_xlpm.m - _xlpm.x - _xlpm.r + 1) + ABS(_xlpm.m - _xlpm.y - _xlpm.c + 1)),
+        _xlpm.ff, _xlfn.LAMBDA(_xlpm.r,_xlpm.c,
+            IF(
+                IF(ISODD(_xlpm.n), _xlpm.f(_xlpm.r, _xlpm.c) &lt;= _xlpm.m, OR(_xlpm.f(_xlpm.r, _xlpm.c, 1, 1) &lt; _xlpm.m, _xlpm.f(_xlpm.r, _xlpm.c, , 1) &lt; _xlpm.m, _xlpm.f(_xlpm.r, _xlpm.c, 1) &lt; _xlpm.m, _xlpm.f(_xlpm.r, _xlpm.c) &lt; _xlpm.m)),
+                "*",
+                ""
+            )
+        ),
+        _xlfn.MAKEARRAY(_xlpm.n, _xlpm.n, _xlpm.ff)
+    )
+)(10)</f>
+        <v/>
+      </c>
+      <c r="AV35" t="str">
+        <v/>
+      </c>
+      <c r="AW35" t="str">
+        <v/>
+      </c>
+      <c r="AX35" t="str">
+        <v/>
+      </c>
+      <c r="AY35" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ35" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA35" t="str">
+        <v/>
+      </c>
+      <c r="BB35" t="str">
+        <v/>
+      </c>
+      <c r="BC35" t="str">
+        <v/>
+      </c>
+      <c r="BD35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU36" t="str">
+        <v/>
+      </c>
+      <c r="AV36" t="str">
+        <v/>
+      </c>
+      <c r="AW36" t="str">
+        <v/>
+      </c>
+      <c r="AX36" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY36" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ36" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA36" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB36" t="str">
+        <v/>
+      </c>
+      <c r="BC36" t="str">
+        <v/>
+      </c>
+      <c r="BD36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU37" t="str">
+        <v/>
+      </c>
+      <c r="AV37" t="str">
+        <v/>
+      </c>
+      <c r="AW37" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX37" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY37" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ37" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA37" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB37" t="str">
+        <v>*</v>
+      </c>
+      <c r="BC37" t="str">
+        <v/>
+      </c>
+      <c r="BD37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="47:56" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AU38" t="str">
+        <v/>
+      </c>
+      <c r="AV38" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW38" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX38" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY38" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ38" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA38" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB38" t="str">
+        <v>*</v>
+      </c>
+      <c r="BC38" t="str">
+        <v>*</v>
+      </c>
+      <c r="BD38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU39" t="str">
+        <v>*</v>
+      </c>
+      <c r="AV39" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW39" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX39" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY39" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ39" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA39" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB39" t="str">
+        <v>*</v>
+      </c>
+      <c r="BC39" t="str">
+        <v>*</v>
+      </c>
+      <c r="BD39" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="40" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU40" t="str">
+        <v>*</v>
+      </c>
+      <c r="AV40" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW40" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX40" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY40" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ40" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA40" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB40" t="str">
+        <v>*</v>
+      </c>
+      <c r="BC40" t="str">
+        <v>*</v>
+      </c>
+      <c r="BD40" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="41" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU41" t="str">
+        <v/>
+      </c>
+      <c r="AV41" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW41" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX41" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY41" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ41" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA41" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB41" t="str">
+        <v>*</v>
+      </c>
+      <c r="BC41" t="str">
+        <v>*</v>
+      </c>
+      <c r="BD41" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU42" t="str">
+        <v/>
+      </c>
+      <c r="AV42" t="str">
+        <v/>
+      </c>
+      <c r="AW42" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX42" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY42" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ42" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA42" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB42" t="str">
+        <v>*</v>
+      </c>
+      <c r="BC42" t="str">
+        <v/>
+      </c>
+      <c r="BD42" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU43" t="str">
+        <v/>
+      </c>
+      <c r="AV43" t="str">
+        <v/>
+      </c>
+      <c r="AW43" t="str">
+        <v/>
+      </c>
+      <c r="AX43" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY43" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ43" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA43" t="str">
+        <v>*</v>
+      </c>
+      <c r="BB43" t="str">
+        <v/>
+      </c>
+      <c r="BC43" t="str">
+        <v/>
+      </c>
+      <c r="BD43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU44" t="str">
+        <v/>
+      </c>
+      <c r="AV44" t="str">
+        <v/>
+      </c>
+      <c r="AW44" t="str">
+        <v/>
+      </c>
+      <c r="AX44" t="str">
+        <v/>
+      </c>
+      <c r="AY44" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ44" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA44" t="str">
+        <v/>
+      </c>
+      <c r="BB44" t="str">
+        <v/>
+      </c>
+      <c r="BC44" t="str">
+        <v/>
+      </c>
+      <c r="BD44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="47:56" x14ac:dyDescent="0.3">
+      <c r="AU48" t="str" cm="1">
+        <f t="array" ref="AU48:AZ53">rhombus(6)</f>
+        <v/>
+      </c>
+      <c r="AV48" t="str">
+        <v/>
+      </c>
+      <c r="AW48" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX48" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY48" t="str">
+        <v/>
+      </c>
+      <c r="AZ48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU49" t="str">
+        <v/>
+      </c>
+      <c r="AV49" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW49" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX49" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY49" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU50" t="str">
+        <v>*</v>
+      </c>
+      <c r="AV50" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW50" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX50" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY50" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ50" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="51" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU51" t="str">
+        <v>*</v>
+      </c>
+      <c r="AV51" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW51" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX51" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY51" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ51" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="52" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU52" t="str">
+        <v/>
+      </c>
+      <c r="AV52" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW52" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX52" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY52" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ52" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU53" t="str">
+        <v/>
+      </c>
+      <c r="AV53" t="str">
+        <v/>
+      </c>
+      <c r="AW53" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX53" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY53" t="str">
+        <v/>
+      </c>
+      <c r="AZ53" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU55" t="str" cm="1">
+        <f t="array" ref="AU55:BA61">rhombus(7)</f>
+        <v/>
+      </c>
+      <c r="AV55" t="str">
+        <v/>
+      </c>
+      <c r="AW55" t="str">
+        <v/>
+      </c>
+      <c r="AX55" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY55" t="str">
+        <v/>
+      </c>
+      <c r="AZ55" t="str">
+        <v/>
+      </c>
+      <c r="BA55" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU56" t="str">
+        <v/>
+      </c>
+      <c r="AV56" t="str">
+        <v/>
+      </c>
+      <c r="AW56" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX56" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY56" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ56" t="str">
+        <v/>
+      </c>
+      <c r="BA56" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU57" t="str">
+        <v/>
+      </c>
+      <c r="AV57" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW57" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX57" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY57" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ57" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA57" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU58" t="str">
+        <v>*</v>
+      </c>
+      <c r="AV58" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW58" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX58" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY58" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ58" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA58" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="59" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU59" t="str">
+        <v/>
+      </c>
+      <c r="AV59" t="str">
+        <v>*</v>
+      </c>
+      <c r="AW59" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX59" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY59" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ59" t="str">
+        <v>*</v>
+      </c>
+      <c r="BA59" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU60" t="str">
+        <v/>
+      </c>
+      <c r="AV60" t="str">
+        <v/>
+      </c>
+      <c r="AW60" t="str">
+        <v>*</v>
+      </c>
+      <c r="AX60" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY60" t="str">
+        <v>*</v>
+      </c>
+      <c r="AZ60" t="str">
+        <v/>
+      </c>
+      <c r="BA60" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="47:53" x14ac:dyDescent="0.3">
+      <c r="AU61" t="str">
+        <v/>
+      </c>
+      <c r="AV61" t="str">
+        <v/>
+      </c>
+      <c r="AW61" t="str">
+        <v/>
+      </c>
+      <c r="AX61" t="str">
+        <v>*</v>
+      </c>
+      <c r="AY61" t="str">
+        <v/>
+      </c>
+      <c r="AZ61" t="str">
+        <v/>
+      </c>
+      <c r="BA61" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finshed my odd version
</commit_message>
<xml_diff>
--- a/CH-77 Character-Based Rhombus.xlsx
+++ b/CH-77 Character-Based Rhombus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B47563-482B-4243-8531-2E003142DFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F555458-9AE7-4D79-AC29-55C60DD79544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -648,6 +648,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1118,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B17870-5941-4C59-8CD8-DDAC51A6FF70}">
-  <dimension ref="C1:Q25"/>
+  <dimension ref="C1:AK90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="Y55" sqref="Y55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,12 +1134,57 @@
     <col min="5" max="5" width="2.44140625" style="4" customWidth="1"/>
     <col min="6" max="17" width="2.44140625" customWidth="1"/>
     <col min="18" max="19" width="2.77734375" customWidth="1"/>
+    <col min="23" max="23" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:17" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:37" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="5">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5">
+        <v>10</v>
+      </c>
+      <c r="M1" s="5">
+        <v>11</v>
+      </c>
+      <c r="N1" s="5">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5">
+        <v>13</v>
+      </c>
+      <c r="P1" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="3:37" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="4"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1144,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:37" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4"/>
       <c r="F3"/>
       <c r="G3"/>
@@ -1158,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:37" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="4"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -1177,8 +1225,58 @@
       <c r="L4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W4" s="1" cm="1">
+        <f t="array" ref="W4:AK11">_xlfn.LET(
+_xlpm.z,15,
+_xlpm.za,INT(_xlpm.z/2)+1,
+_xlpm.q,_xlfn.DROP(_xlfn.REDUCE(0,_xlfn.SEQUENCE(_xlpm.za,1,1,2),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.SEQUENCE(1,_xlpm.v,_xlpm.za-INT(_xlpm.v/2),1)))),1),
+_xlpm.q)</f>
+        <v>8</v>
+      </c>
+      <c r="X4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AB4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AE4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AF4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AG4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AH4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK4" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="3:37" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="4"/>
       <c r="F5"/>
       <c r="G5" s="1" t="s">
@@ -1202,8 +1300,53 @@
       <c r="M5" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W5" s="1">
+        <v>7</v>
+      </c>
+      <c r="X5" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AB5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AE5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AF5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AG5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AH5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK5" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="3:37" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E6" s="4"/>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -1232,8 +1375,53 @@
       <c r="N6" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:17" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W6" s="1">
+        <v>6</v>
+      </c>
+      <c r="X6" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AE6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AF6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AG6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AH6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK6" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="3:37" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,8 +1455,53 @@
       <c r="O7" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W7" s="1">
+        <v>5</v>
+      </c>
+      <c r="X7" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>11</v>
+      </c>
+      <c r="AD7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AE7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AF7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AG7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AH7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK7" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1308,8 +1541,53 @@
       <c r="P8" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <v>5</v>
+      </c>
+      <c r="Y8">
+        <v>6</v>
+      </c>
+      <c r="Z8">
+        <v>7</v>
+      </c>
+      <c r="AA8">
+        <v>8</v>
+      </c>
+      <c r="AB8">
+        <v>9</v>
+      </c>
+      <c r="AC8">
+        <v>10</v>
+      </c>
+      <c r="AD8">
+        <v>11</v>
+      </c>
+      <c r="AE8">
+        <v>12</v>
+      </c>
+      <c r="AF8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AG8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AH8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK8" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1355,8 +1633,53 @@
       <c r="Q9" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W9">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <v>5</v>
+      </c>
+      <c r="Z9">
+        <v>6</v>
+      </c>
+      <c r="AA9">
+        <v>7</v>
+      </c>
+      <c r="AB9">
+        <v>8</v>
+      </c>
+      <c r="AC9">
+        <v>9</v>
+      </c>
+      <c r="AD9">
+        <v>10</v>
+      </c>
+      <c r="AE9">
+        <v>11</v>
+      </c>
+      <c r="AF9">
+        <v>12</v>
+      </c>
+      <c r="AG9">
+        <v>13</v>
+      </c>
+      <c r="AH9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1396,8 +1719,53 @@
       <c r="P10" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W10">
+        <v>2</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>4</v>
+      </c>
+      <c r="Z10">
+        <v>5</v>
+      </c>
+      <c r="AA10">
+        <v>6</v>
+      </c>
+      <c r="AB10">
+        <v>7</v>
+      </c>
+      <c r="AC10">
+        <v>8</v>
+      </c>
+      <c r="AD10">
+        <v>9</v>
+      </c>
+      <c r="AE10">
+        <v>10</v>
+      </c>
+      <c r="AF10">
+        <v>11</v>
+      </c>
+      <c r="AG10">
+        <v>12</v>
+      </c>
+      <c r="AH10">
+        <v>13</v>
+      </c>
+      <c r="AI10">
+        <v>14</v>
+      </c>
+      <c r="AJ10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK10" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,8 +1799,53 @@
       <c r="O11" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>2</v>
+      </c>
+      <c r="Y11">
+        <v>3</v>
+      </c>
+      <c r="Z11">
+        <v>4</v>
+      </c>
+      <c r="AA11">
+        <v>5</v>
+      </c>
+      <c r="AB11">
+        <v>6</v>
+      </c>
+      <c r="AC11">
+        <v>7</v>
+      </c>
+      <c r="AD11">
+        <v>8</v>
+      </c>
+      <c r="AE11">
+        <v>9</v>
+      </c>
+      <c r="AF11">
+        <v>10</v>
+      </c>
+      <c r="AG11">
+        <v>11</v>
+      </c>
+      <c r="AH11">
+        <v>12</v>
+      </c>
+      <c r="AI11">
+        <v>13</v>
+      </c>
+      <c r="AJ11">
+        <v>14</v>
+      </c>
+      <c r="AK11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>0</v>
@@ -1463,7 +1876,7 @@
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F13" s="3"/>
       <c r="G13" s="1" t="s">
         <v>0</v>
@@ -1487,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
@@ -1506,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="1"/>
@@ -1521,7 +1934,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="3:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:37" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="1"/>
@@ -1532,40 +1945,2229 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="H25" s="3"/>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C18" t="str" cm="1">
+        <f t="array" ref="C18:Q32">_xlfn.MAKEARRAY(15,15,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=7,_xlpm.r-1+_xlpm.c-1&gt;=7,_xlpm.r-1+_xlpm.c-1&lt;=21,_xlpm.r-1-_xlpm.c+1&gt;=-7),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <v>*</v>
+      </c>
+      <c r="K18" t="str">
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
+      <c r="Q18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <v>*</v>
+      </c>
+      <c r="J19" t="str">
+        <v>*</v>
+      </c>
+      <c r="K19" t="str">
+        <v>*</v>
+      </c>
+      <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
+      <c r="Q19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C20" t="str">
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <v>*</v>
+      </c>
+      <c r="I20" t="str">
+        <v>*</v>
+      </c>
+      <c r="J20" t="str">
+        <v>*</v>
+      </c>
+      <c r="K20" t="str">
+        <v>*</v>
+      </c>
+      <c r="L20" t="str">
+        <v>*</v>
+      </c>
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <v/>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
+      <c r="Q20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" t="str">
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <v/>
+      </c>
+      <c r="E21" t="str">
+        <v/>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v>*</v>
+      </c>
+      <c r="H21" t="str">
+        <v>*</v>
+      </c>
+      <c r="I21" t="str">
+        <v>*</v>
+      </c>
+      <c r="J21" t="str">
+        <v>*</v>
+      </c>
+      <c r="K21" t="str">
+        <v>*</v>
+      </c>
+      <c r="L21" t="str">
+        <v>*</v>
+      </c>
+      <c r="M21" t="str">
+        <v>*</v>
+      </c>
+      <c r="N21" t="str">
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v/>
+      </c>
+      <c r="Q21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C22" t="str">
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <v>*</v>
+      </c>
+      <c r="G22" t="str">
+        <v>*</v>
+      </c>
+      <c r="H22" t="str">
+        <v>*</v>
+      </c>
+      <c r="I22" t="str">
+        <v>*</v>
+      </c>
+      <c r="J22" t="str">
+        <v>*</v>
+      </c>
+      <c r="K22" t="str">
+        <v>*</v>
+      </c>
+      <c r="L22" t="str">
+        <v>*</v>
+      </c>
+      <c r="M22" t="str">
+        <v>*</v>
+      </c>
+      <c r="N22" t="str">
+        <v>*</v>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
+      <c r="Q22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <v>*</v>
+      </c>
+      <c r="F23" t="str">
+        <v>*</v>
+      </c>
+      <c r="G23" t="str">
+        <v>*</v>
+      </c>
+      <c r="H23" t="str">
+        <v>*</v>
+      </c>
+      <c r="I23" t="str">
+        <v>*</v>
+      </c>
+      <c r="J23" t="str">
+        <v>*</v>
+      </c>
+      <c r="K23" t="str">
+        <v>*</v>
+      </c>
+      <c r="L23" t="str">
+        <v>*</v>
+      </c>
+      <c r="M23" t="str">
+        <v>*</v>
+      </c>
+      <c r="N23" t="str">
+        <v>*</v>
+      </c>
+      <c r="O23" t="str">
+        <v>*</v>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C24" t="str">
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <v>*</v>
+      </c>
+      <c r="E24" t="str">
+        <v>*</v>
+      </c>
+      <c r="F24" t="str">
+        <v>*</v>
+      </c>
+      <c r="G24" t="str">
+        <v>*</v>
+      </c>
+      <c r="H24" t="str">
+        <v>*</v>
+      </c>
+      <c r="I24" t="str">
+        <v>*</v>
+      </c>
+      <c r="J24" t="str">
+        <v>*</v>
+      </c>
+      <c r="K24" t="str">
+        <v>*</v>
+      </c>
+      <c r="L24" t="str">
+        <v>*</v>
+      </c>
+      <c r="M24" t="str">
+        <v>*</v>
+      </c>
+      <c r="N24" t="str">
+        <v>*</v>
+      </c>
+      <c r="O24" t="str">
+        <v>*</v>
+      </c>
+      <c r="P24" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <v>*</v>
+      </c>
+      <c r="D25" t="str">
+        <v>*</v>
+      </c>
+      <c r="E25" t="str">
+        <v>*</v>
+      </c>
+      <c r="F25" t="str">
+        <v>*</v>
+      </c>
+      <c r="G25" t="str">
+        <v>*</v>
+      </c>
+      <c r="H25" t="str">
+        <v>*</v>
+      </c>
+      <c r="I25" t="str">
+        <v>*</v>
+      </c>
+      <c r="J25" t="str">
+        <v>*</v>
+      </c>
+      <c r="K25" t="str">
+        <v>*</v>
+      </c>
+      <c r="L25" t="str">
+        <v>*</v>
+      </c>
+      <c r="M25" t="str">
+        <v>*</v>
+      </c>
+      <c r="N25" t="str">
+        <v>*</v>
+      </c>
+      <c r="O25" t="str">
+        <v>*</v>
+      </c>
+      <c r="P25" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C26" t="str">
+        <v/>
+      </c>
+      <c r="D26" t="str">
+        <v>*</v>
+      </c>
+      <c r="E26" t="str">
+        <v>*</v>
+      </c>
+      <c r="F26" t="str">
+        <v>*</v>
+      </c>
+      <c r="G26" t="str">
+        <v>*</v>
+      </c>
+      <c r="H26" t="str">
+        <v>*</v>
+      </c>
+      <c r="I26" t="str">
+        <v>*</v>
+      </c>
+      <c r="J26" t="str">
+        <v>*</v>
+      </c>
+      <c r="K26" t="str">
+        <v>*</v>
+      </c>
+      <c r="L26" t="str">
+        <v>*</v>
+      </c>
+      <c r="M26" t="str">
+        <v>*</v>
+      </c>
+      <c r="N26" t="str">
+        <v>*</v>
+      </c>
+      <c r="O26" t="str">
+        <v>*</v>
+      </c>
+      <c r="P26" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C27" t="str">
+        <v/>
+      </c>
+      <c r="D27" t="str">
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <v>*</v>
+      </c>
+      <c r="F27" t="str">
+        <v>*</v>
+      </c>
+      <c r="G27" t="str">
+        <v>*</v>
+      </c>
+      <c r="H27" t="str">
+        <v>*</v>
+      </c>
+      <c r="I27" t="str">
+        <v>*</v>
+      </c>
+      <c r="J27" t="str">
+        <v>*</v>
+      </c>
+      <c r="K27" t="str">
+        <v>*</v>
+      </c>
+      <c r="L27" t="str">
+        <v>*</v>
+      </c>
+      <c r="M27" t="str">
+        <v>*</v>
+      </c>
+      <c r="N27" t="str">
+        <v>*</v>
+      </c>
+      <c r="O27" t="str">
+        <v>*</v>
+      </c>
+      <c r="P27" t="str">
+        <v/>
+      </c>
+      <c r="Q27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C28" t="str">
+        <v/>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <v/>
+      </c>
+      <c r="F28" t="str">
+        <v>*</v>
+      </c>
+      <c r="G28" t="str">
+        <v>*</v>
+      </c>
+      <c r="H28" t="str">
+        <v>*</v>
+      </c>
+      <c r="I28" t="str">
+        <v>*</v>
+      </c>
+      <c r="J28" t="str">
+        <v>*</v>
+      </c>
+      <c r="K28" t="str">
+        <v>*</v>
+      </c>
+      <c r="L28" t="str">
+        <v>*</v>
+      </c>
+      <c r="M28" t="str">
+        <v>*</v>
+      </c>
+      <c r="N28" t="str">
+        <v>*</v>
+      </c>
+      <c r="O28" t="str">
+        <v/>
+      </c>
+      <c r="P28" t="str">
+        <v/>
+      </c>
+      <c r="Q28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C29" t="str">
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29" t="str">
+        <v/>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v>*</v>
+      </c>
+      <c r="H29" t="str">
+        <v>*</v>
+      </c>
+      <c r="I29" t="str">
+        <v>*</v>
+      </c>
+      <c r="J29" t="str">
+        <v>*</v>
+      </c>
+      <c r="K29" t="str">
+        <v>*</v>
+      </c>
+      <c r="L29" t="str">
+        <v>*</v>
+      </c>
+      <c r="M29" t="str">
+        <v>*</v>
+      </c>
+      <c r="N29" t="str">
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <v/>
+      </c>
+      <c r="P29" t="str">
+        <v/>
+      </c>
+      <c r="Q29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+      <c r="G30" t="str">
+        <v/>
+      </c>
+      <c r="H30" t="str">
+        <v>*</v>
+      </c>
+      <c r="I30" t="str">
+        <v>*</v>
+      </c>
+      <c r="J30" t="str">
+        <v>*</v>
+      </c>
+      <c r="K30" t="str">
+        <v>*</v>
+      </c>
+      <c r="L30" t="str">
+        <v>*</v>
+      </c>
+      <c r="M30" t="str">
+        <v/>
+      </c>
+      <c r="N30" t="str">
+        <v/>
+      </c>
+      <c r="O30" t="str">
+        <v/>
+      </c>
+      <c r="P30" t="str">
+        <v/>
+      </c>
+      <c r="Q30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <v/>
+      </c>
+      <c r="E31" t="str">
+        <v/>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="str">
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <v>*</v>
+      </c>
+      <c r="J31" t="str">
+        <v>*</v>
+      </c>
+      <c r="K31" t="str">
+        <v>*</v>
+      </c>
+      <c r="L31" t="str">
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <v/>
+      </c>
+      <c r="N31" t="str">
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <v/>
+      </c>
+      <c r="P31" t="str">
+        <v/>
+      </c>
+      <c r="Q31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+      <c r="H32" t="str">
+        <v/>
+      </c>
+      <c r="I32" t="str">
+        <v/>
+      </c>
+      <c r="J32" t="str">
+        <v>*</v>
+      </c>
+      <c r="K32" t="str">
+        <v/>
+      </c>
+      <c r="L32" t="str">
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <v/>
+      </c>
+      <c r="N32" t="str">
+        <v/>
+      </c>
+      <c r="O32" t="str">
+        <v/>
+      </c>
+      <c r="P32" t="str">
+        <v/>
+      </c>
+      <c r="Q32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C34" t="str" cm="1">
+        <f t="array" ref="C34:I40">_xlfn.MAKEARRAY(7,7,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=3,_xlpm.r-1+_xlpm.c-1&gt;=3,_xlpm.r-1+_xlpm.c-1&lt;=9,_xlpm.r-1-_xlpm.c+1&gt;=-3),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v/>
+      </c>
+      <c r="E34" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <v>*</v>
+      </c>
+      <c r="G34" t="str">
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <v/>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <v/>
+      </c>
+      <c r="E35" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F35" t="str">
+        <v>*</v>
+      </c>
+      <c r="G35" t="str">
+        <v>*</v>
+      </c>
+      <c r="H35" t="str">
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C36" t="str">
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <v>*</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F36" t="str">
+        <v>*</v>
+      </c>
+      <c r="G36" t="str">
+        <v>*</v>
+      </c>
+      <c r="H36" t="str">
+        <v>*</v>
+      </c>
+      <c r="I36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C37" t="str">
+        <v>*</v>
+      </c>
+      <c r="D37" t="str">
+        <v>*</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F37" t="str">
+        <v>*</v>
+      </c>
+      <c r="G37" t="str">
+        <v>*</v>
+      </c>
+      <c r="H37" t="str">
+        <v>*</v>
+      </c>
+      <c r="I37" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v>*</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F38" t="str">
+        <v>*</v>
+      </c>
+      <c r="G38" t="str">
+        <v>*</v>
+      </c>
+      <c r="H38" t="str">
+        <v>*</v>
+      </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C39" t="str">
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <v/>
+      </c>
+      <c r="E39" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F39" t="str">
+        <v>*</v>
+      </c>
+      <c r="G39" t="str">
+        <v>*</v>
+      </c>
+      <c r="H39" t="str">
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C40" t="str">
+        <v/>
+      </c>
+      <c r="D40" t="str">
+        <v/>
+      </c>
+      <c r="E40" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F40" t="str">
+        <v>*</v>
+      </c>
+      <c r="G40" t="str">
+        <v/>
+      </c>
+      <c r="H40" t="str">
+        <v/>
+      </c>
+      <c r="I40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C43" t="str" cm="1">
+        <f t="array" ref="C43:K51">_xlfn.MAKEARRAY(9,9,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=4,_xlpm.r-1+_xlpm.c-1&gt;=4,_xlpm.r-1+_xlpm.c-1&lt;=12,_xlpm.r-1-_xlpm.c+1&gt;=-4),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F43" t="str">
+        <v/>
+      </c>
+      <c r="G43" t="str">
+        <v>*</v>
+      </c>
+      <c r="H43" t="str">
+        <v/>
+      </c>
+      <c r="I43" t="str">
+        <v/>
+      </c>
+      <c r="J43" t="str">
+        <v/>
+      </c>
+      <c r="K43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C44" t="str">
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <v/>
+      </c>
+      <c r="E44" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F44" t="str">
+        <v>*</v>
+      </c>
+      <c r="G44" t="str">
+        <v>*</v>
+      </c>
+      <c r="H44" t="str">
+        <v>*</v>
+      </c>
+      <c r="I44" t="str">
+        <v/>
+      </c>
+      <c r="J44" t="str">
+        <v/>
+      </c>
+      <c r="K44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C45" t="str">
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F45" t="str">
+        <v>*</v>
+      </c>
+      <c r="G45" t="str">
+        <v>*</v>
+      </c>
+      <c r="H45" t="str">
+        <v>*</v>
+      </c>
+      <c r="I45" t="str">
+        <v>*</v>
+      </c>
+      <c r="J45" t="str">
+        <v/>
+      </c>
+      <c r="K45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C46" t="str">
+        <v/>
+      </c>
+      <c r="D46" t="str">
+        <v>*</v>
+      </c>
+      <c r="E46" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F46" t="str">
+        <v>*</v>
+      </c>
+      <c r="G46" t="str">
+        <v>*</v>
+      </c>
+      <c r="H46" t="str">
+        <v>*</v>
+      </c>
+      <c r="I46" t="str">
+        <v>*</v>
+      </c>
+      <c r="J46" t="str">
+        <v>*</v>
+      </c>
+      <c r="K46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C47" t="str">
+        <v>*</v>
+      </c>
+      <c r="D47" t="str">
+        <v>*</v>
+      </c>
+      <c r="E47" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F47" t="str">
+        <v>*</v>
+      </c>
+      <c r="G47" t="str">
+        <v>*</v>
+      </c>
+      <c r="H47" t="str">
+        <v>*</v>
+      </c>
+      <c r="I47" t="str">
+        <v>*</v>
+      </c>
+      <c r="J47" t="str">
+        <v>*</v>
+      </c>
+      <c r="K47" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C48" t="str">
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <v>*</v>
+      </c>
+      <c r="E48" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F48" t="str">
+        <v>*</v>
+      </c>
+      <c r="G48" t="str">
+        <v>*</v>
+      </c>
+      <c r="H48" t="str">
+        <v>*</v>
+      </c>
+      <c r="I48" t="str">
+        <v>*</v>
+      </c>
+      <c r="J48" t="str">
+        <v>*</v>
+      </c>
+      <c r="K48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C49" t="str">
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+      <c r="E49" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F49" t="str">
+        <v>*</v>
+      </c>
+      <c r="G49" t="str">
+        <v>*</v>
+      </c>
+      <c r="H49" t="str">
+        <v>*</v>
+      </c>
+      <c r="I49" t="str">
+        <v>*</v>
+      </c>
+      <c r="J49" t="str">
+        <v/>
+      </c>
+      <c r="K49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C50" t="str">
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <v/>
+      </c>
+      <c r="E50" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F50" t="str">
+        <v>*</v>
+      </c>
+      <c r="G50" t="str">
+        <v>*</v>
+      </c>
+      <c r="H50" t="str">
+        <v>*</v>
+      </c>
+      <c r="I50" t="str">
+        <v/>
+      </c>
+      <c r="J50" t="str">
+        <v/>
+      </c>
+      <c r="K50" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C51" t="str">
+        <v/>
+      </c>
+      <c r="D51" t="str">
+        <v/>
+      </c>
+      <c r="E51" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F51" t="str">
+        <v/>
+      </c>
+      <c r="G51" t="str">
+        <v>*</v>
+      </c>
+      <c r="H51" t="str">
+        <v/>
+      </c>
+      <c r="I51" t="str">
+        <v/>
+      </c>
+      <c r="J51" t="str">
+        <v/>
+      </c>
+      <c r="K51" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C54" t="str" cm="1">
+        <f t="array" ref="C54:M64">_xlfn.MAKEARRAY(11,11,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=5,_xlpm.r-1+_xlpm.c-1&gt;=5,_xlpm.r-1+_xlpm.c-1&lt;=15,_xlpm.r-1-_xlpm.c+1&gt;=-5),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D54" t="str">
+        <v/>
+      </c>
+      <c r="E54" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F54" t="str">
+        <v/>
+      </c>
+      <c r="G54" t="str">
+        <v/>
+      </c>
+      <c r="H54" t="str">
+        <v>*</v>
+      </c>
+      <c r="I54" t="str">
+        <v/>
+      </c>
+      <c r="J54" t="str">
+        <v/>
+      </c>
+      <c r="K54" t="str">
+        <v/>
+      </c>
+      <c r="L54" t="str">
+        <v/>
+      </c>
+      <c r="M54" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C55" t="str">
+        <v/>
+      </c>
+      <c r="D55" t="str">
+        <v/>
+      </c>
+      <c r="E55" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F55" t="str">
+        <v/>
+      </c>
+      <c r="G55" t="str">
+        <v>*</v>
+      </c>
+      <c r="H55" t="str">
+        <v>*</v>
+      </c>
+      <c r="I55" t="str">
+        <v>*</v>
+      </c>
+      <c r="J55" t="str">
+        <v/>
+      </c>
+      <c r="K55" t="str">
+        <v/>
+      </c>
+      <c r="L55" t="str">
+        <v/>
+      </c>
+      <c r="M55" t="str">
+        <v/>
+      </c>
+      <c r="V55">
+        <v>3</v>
+      </c>
+      <c r="W55">
+        <v>3</v>
+      </c>
+      <c r="Y55" cm="1">
+        <f t="array" ref="Y55:Z55">LINEST(W55:W61,V55:V61)</f>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="Z55">
+        <v>-1.4999999999999982</v>
+      </c>
+    </row>
+    <row r="56" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C56" t="str">
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <v/>
+      </c>
+      <c r="E56" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F56" t="str">
+        <v>*</v>
+      </c>
+      <c r="G56" t="str">
+        <v>*</v>
+      </c>
+      <c r="H56" t="str">
+        <v>*</v>
+      </c>
+      <c r="I56" t="str">
+        <v>*</v>
+      </c>
+      <c r="J56" t="str">
+        <v>*</v>
+      </c>
+      <c r="K56" t="str">
+        <v/>
+      </c>
+      <c r="L56" t="str">
+        <v/>
+      </c>
+      <c r="M56" t="str">
+        <v/>
+      </c>
+      <c r="V56">
+        <v>5</v>
+      </c>
+      <c r="W56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C57" t="str">
+        <v/>
+      </c>
+      <c r="D57" t="str">
+        <v/>
+      </c>
+      <c r="E57" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F57" t="str">
+        <v>*</v>
+      </c>
+      <c r="G57" t="str">
+        <v>*</v>
+      </c>
+      <c r="H57" t="str">
+        <v>*</v>
+      </c>
+      <c r="I57" t="str">
+        <v>*</v>
+      </c>
+      <c r="J57" t="str">
+        <v>*</v>
+      </c>
+      <c r="K57" t="str">
+        <v>*</v>
+      </c>
+      <c r="L57" t="str">
+        <v/>
+      </c>
+      <c r="M57" t="str">
+        <v/>
+      </c>
+      <c r="V57">
+        <v>7</v>
+      </c>
+      <c r="W57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C58" t="str">
+        <v/>
+      </c>
+      <c r="D58" t="str">
+        <v>*</v>
+      </c>
+      <c r="E58" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F58" t="str">
+        <v>*</v>
+      </c>
+      <c r="G58" t="str">
+        <v>*</v>
+      </c>
+      <c r="H58" t="str">
+        <v>*</v>
+      </c>
+      <c r="I58" t="str">
+        <v>*</v>
+      </c>
+      <c r="J58" t="str">
+        <v>*</v>
+      </c>
+      <c r="K58" t="str">
+        <v>*</v>
+      </c>
+      <c r="L58" t="str">
+        <v>*</v>
+      </c>
+      <c r="M58" t="str">
+        <v/>
+      </c>
+      <c r="V58">
+        <v>9</v>
+      </c>
+      <c r="W58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C59" t="str">
+        <v>*</v>
+      </c>
+      <c r="D59" t="str">
+        <v>*</v>
+      </c>
+      <c r="E59" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F59" t="str">
+        <v>*</v>
+      </c>
+      <c r="G59" t="str">
+        <v>*</v>
+      </c>
+      <c r="H59" t="str">
+        <v>*</v>
+      </c>
+      <c r="I59" t="str">
+        <v>*</v>
+      </c>
+      <c r="J59" t="str">
+        <v>*</v>
+      </c>
+      <c r="K59" t="str">
+        <v>*</v>
+      </c>
+      <c r="L59" t="str">
+        <v>*</v>
+      </c>
+      <c r="M59" t="str">
+        <v>*</v>
+      </c>
+      <c r="V59">
+        <v>11</v>
+      </c>
+      <c r="W59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C60" t="str">
+        <v/>
+      </c>
+      <c r="D60" t="str">
+        <v>*</v>
+      </c>
+      <c r="E60" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F60" t="str">
+        <v>*</v>
+      </c>
+      <c r="G60" t="str">
+        <v>*</v>
+      </c>
+      <c r="H60" t="str">
+        <v>*</v>
+      </c>
+      <c r="I60" t="str">
+        <v>*</v>
+      </c>
+      <c r="J60" t="str">
+        <v>*</v>
+      </c>
+      <c r="K60" t="str">
+        <v>*</v>
+      </c>
+      <c r="L60" t="str">
+        <v>*</v>
+      </c>
+      <c r="M60" t="str">
+        <v/>
+      </c>
+      <c r="V60">
+        <v>13</v>
+      </c>
+      <c r="W60">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C61" t="str">
+        <v/>
+      </c>
+      <c r="D61" t="str">
+        <v/>
+      </c>
+      <c r="E61" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F61" t="str">
+        <v>*</v>
+      </c>
+      <c r="G61" t="str">
+        <v>*</v>
+      </c>
+      <c r="H61" t="str">
+        <v>*</v>
+      </c>
+      <c r="I61" t="str">
+        <v>*</v>
+      </c>
+      <c r="J61" t="str">
+        <v>*</v>
+      </c>
+      <c r="K61" t="str">
+        <v>*</v>
+      </c>
+      <c r="L61" t="str">
+        <v/>
+      </c>
+      <c r="M61" t="str">
+        <v/>
+      </c>
+      <c r="V61">
+        <v>15</v>
+      </c>
+      <c r="W61">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C62" t="str">
+        <v/>
+      </c>
+      <c r="D62" t="str">
+        <v/>
+      </c>
+      <c r="E62" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F62" t="str">
+        <v>*</v>
+      </c>
+      <c r="G62" t="str">
+        <v>*</v>
+      </c>
+      <c r="H62" t="str">
+        <v>*</v>
+      </c>
+      <c r="I62" t="str">
+        <v>*</v>
+      </c>
+      <c r="J62" t="str">
+        <v>*</v>
+      </c>
+      <c r="K62" t="str">
+        <v/>
+      </c>
+      <c r="L62" t="str">
+        <v/>
+      </c>
+      <c r="M62" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C63" t="str">
+        <v/>
+      </c>
+      <c r="D63" t="str">
+        <v/>
+      </c>
+      <c r="E63" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F63" t="str">
+        <v/>
+      </c>
+      <c r="G63" t="str">
+        <v>*</v>
+      </c>
+      <c r="H63" t="str">
+        <v>*</v>
+      </c>
+      <c r="I63" t="str">
+        <v>*</v>
+      </c>
+      <c r="J63" t="str">
+        <v/>
+      </c>
+      <c r="K63" t="str">
+        <v/>
+      </c>
+      <c r="L63" t="str">
+        <v/>
+      </c>
+      <c r="M63" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C64" t="str">
+        <v/>
+      </c>
+      <c r="D64" t="str">
+        <v/>
+      </c>
+      <c r="E64" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F64" t="str">
+        <v/>
+      </c>
+      <c r="G64" t="str">
+        <v/>
+      </c>
+      <c r="H64" t="str">
+        <v>*</v>
+      </c>
+      <c r="I64" t="str">
+        <v/>
+      </c>
+      <c r="J64" t="str">
+        <v/>
+      </c>
+      <c r="K64" t="str">
+        <v/>
+      </c>
+      <c r="L64" t="str">
+        <v/>
+      </c>
+      <c r="M64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C67" t="str" cm="1">
+        <f t="array" ref="C67:O79">_xlfn.MAKEARRAY(13,13,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=6,_xlpm.r-1+_xlpm.c-1&gt;=6,_xlpm.r-1+_xlpm.c-1&lt;=18,_xlpm.r-1-_xlpm.c+1&gt;=-6),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D67" t="str">
+        <v/>
+      </c>
+      <c r="E67" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F67" t="str">
+        <v/>
+      </c>
+      <c r="G67" t="str">
+        <v/>
+      </c>
+      <c r="H67" t="str">
+        <v/>
+      </c>
+      <c r="I67" t="str">
+        <v>*</v>
+      </c>
+      <c r="J67" t="str">
+        <v/>
+      </c>
+      <c r="K67" t="str">
+        <v/>
+      </c>
+      <c r="L67" t="str">
+        <v/>
+      </c>
+      <c r="M67" t="str">
+        <v/>
+      </c>
+      <c r="N67" t="str">
+        <v/>
+      </c>
+      <c r="O67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C68" t="str">
+        <v/>
+      </c>
+      <c r="D68" t="str">
+        <v/>
+      </c>
+      <c r="E68" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F68" t="str">
+        <v/>
+      </c>
+      <c r="G68" t="str">
+        <v/>
+      </c>
+      <c r="H68" t="str">
+        <v>*</v>
+      </c>
+      <c r="I68" t="str">
+        <v>*</v>
+      </c>
+      <c r="J68" t="str">
+        <v>*</v>
+      </c>
+      <c r="K68" t="str">
+        <v/>
+      </c>
+      <c r="L68" t="str">
+        <v/>
+      </c>
+      <c r="M68" t="str">
+        <v/>
+      </c>
+      <c r="N68" t="str">
+        <v/>
+      </c>
+      <c r="O68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C69" t="str">
+        <v/>
+      </c>
+      <c r="D69" t="str">
+        <v/>
+      </c>
+      <c r="E69" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F69" t="str">
+        <v/>
+      </c>
+      <c r="G69" t="str">
+        <v>*</v>
+      </c>
+      <c r="H69" t="str">
+        <v>*</v>
+      </c>
+      <c r="I69" t="str">
+        <v>*</v>
+      </c>
+      <c r="J69" t="str">
+        <v>*</v>
+      </c>
+      <c r="K69" t="str">
+        <v>*</v>
+      </c>
+      <c r="L69" t="str">
+        <v/>
+      </c>
+      <c r="M69" t="str">
+        <v/>
+      </c>
+      <c r="N69" t="str">
+        <v/>
+      </c>
+      <c r="O69" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C70" t="str">
+        <v/>
+      </c>
+      <c r="D70" t="str">
+        <v/>
+      </c>
+      <c r="E70" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F70" t="str">
+        <v>*</v>
+      </c>
+      <c r="G70" t="str">
+        <v>*</v>
+      </c>
+      <c r="H70" t="str">
+        <v>*</v>
+      </c>
+      <c r="I70" t="str">
+        <v>*</v>
+      </c>
+      <c r="J70" t="str">
+        <v>*</v>
+      </c>
+      <c r="K70" t="str">
+        <v>*</v>
+      </c>
+      <c r="L70" t="str">
+        <v>*</v>
+      </c>
+      <c r="M70" t="str">
+        <v/>
+      </c>
+      <c r="N70" t="str">
+        <v/>
+      </c>
+      <c r="O70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C71" t="str">
+        <v/>
+      </c>
+      <c r="D71" t="str">
+        <v/>
+      </c>
+      <c r="E71" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F71" t="str">
+        <v>*</v>
+      </c>
+      <c r="G71" t="str">
+        <v>*</v>
+      </c>
+      <c r="H71" t="str">
+        <v>*</v>
+      </c>
+      <c r="I71" t="str">
+        <v>*</v>
+      </c>
+      <c r="J71" t="str">
+        <v>*</v>
+      </c>
+      <c r="K71" t="str">
+        <v>*</v>
+      </c>
+      <c r="L71" t="str">
+        <v>*</v>
+      </c>
+      <c r="M71" t="str">
+        <v>*</v>
+      </c>
+      <c r="N71" t="str">
+        <v/>
+      </c>
+      <c r="O71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C72" t="str">
+        <v/>
+      </c>
+      <c r="D72" t="str">
+        <v>*</v>
+      </c>
+      <c r="E72" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F72" t="str">
+        <v>*</v>
+      </c>
+      <c r="G72" t="str">
+        <v>*</v>
+      </c>
+      <c r="H72" t="str">
+        <v>*</v>
+      </c>
+      <c r="I72" t="str">
+        <v>*</v>
+      </c>
+      <c r="J72" t="str">
+        <v>*</v>
+      </c>
+      <c r="K72" t="str">
+        <v>*</v>
+      </c>
+      <c r="L72" t="str">
+        <v>*</v>
+      </c>
+      <c r="M72" t="str">
+        <v>*</v>
+      </c>
+      <c r="N72" t="str">
+        <v>*</v>
+      </c>
+      <c r="O72" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C73" t="str">
+        <v>*</v>
+      </c>
+      <c r="D73" t="str">
+        <v>*</v>
+      </c>
+      <c r="E73" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F73" t="str">
+        <v>*</v>
+      </c>
+      <c r="G73" t="str">
+        <v>*</v>
+      </c>
+      <c r="H73" t="str">
+        <v>*</v>
+      </c>
+      <c r="I73" t="str">
+        <v>*</v>
+      </c>
+      <c r="J73" t="str">
+        <v>*</v>
+      </c>
+      <c r="K73" t="str">
+        <v>*</v>
+      </c>
+      <c r="L73" t="str">
+        <v>*</v>
+      </c>
+      <c r="M73" t="str">
+        <v>*</v>
+      </c>
+      <c r="N73" t="str">
+        <v>*</v>
+      </c>
+      <c r="O73" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="74" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C74" t="str">
+        <v/>
+      </c>
+      <c r="D74" t="str">
+        <v>*</v>
+      </c>
+      <c r="E74" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F74" t="str">
+        <v>*</v>
+      </c>
+      <c r="G74" t="str">
+        <v>*</v>
+      </c>
+      <c r="H74" t="str">
+        <v>*</v>
+      </c>
+      <c r="I74" t="str">
+        <v>*</v>
+      </c>
+      <c r="J74" t="str">
+        <v>*</v>
+      </c>
+      <c r="K74" t="str">
+        <v>*</v>
+      </c>
+      <c r="L74" t="str">
+        <v>*</v>
+      </c>
+      <c r="M74" t="str">
+        <v>*</v>
+      </c>
+      <c r="N74" t="str">
+        <v>*</v>
+      </c>
+      <c r="O74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C75" t="str">
+        <v/>
+      </c>
+      <c r="D75" t="str">
+        <v/>
+      </c>
+      <c r="E75" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F75" t="str">
+        <v>*</v>
+      </c>
+      <c r="G75" t="str">
+        <v>*</v>
+      </c>
+      <c r="H75" t="str">
+        <v>*</v>
+      </c>
+      <c r="I75" t="str">
+        <v>*</v>
+      </c>
+      <c r="J75" t="str">
+        <v>*</v>
+      </c>
+      <c r="K75" t="str">
+        <v>*</v>
+      </c>
+      <c r="L75" t="str">
+        <v>*</v>
+      </c>
+      <c r="M75" t="str">
+        <v>*</v>
+      </c>
+      <c r="N75" t="str">
+        <v/>
+      </c>
+      <c r="O75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C76" t="str">
+        <v/>
+      </c>
+      <c r="D76" t="str">
+        <v/>
+      </c>
+      <c r="E76" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F76" t="str">
+        <v>*</v>
+      </c>
+      <c r="G76" t="str">
+        <v>*</v>
+      </c>
+      <c r="H76" t="str">
+        <v>*</v>
+      </c>
+      <c r="I76" t="str">
+        <v>*</v>
+      </c>
+      <c r="J76" t="str">
+        <v>*</v>
+      </c>
+      <c r="K76" t="str">
+        <v>*</v>
+      </c>
+      <c r="L76" t="str">
+        <v>*</v>
+      </c>
+      <c r="M76" t="str">
+        <v/>
+      </c>
+      <c r="N76" t="str">
+        <v/>
+      </c>
+      <c r="O76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C77" t="str">
+        <v/>
+      </c>
+      <c r="D77" t="str">
+        <v/>
+      </c>
+      <c r="E77" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F77" t="str">
+        <v/>
+      </c>
+      <c r="G77" t="str">
+        <v>*</v>
+      </c>
+      <c r="H77" t="str">
+        <v>*</v>
+      </c>
+      <c r="I77" t="str">
+        <v>*</v>
+      </c>
+      <c r="J77" t="str">
+        <v>*</v>
+      </c>
+      <c r="K77" t="str">
+        <v>*</v>
+      </c>
+      <c r="L77" t="str">
+        <v/>
+      </c>
+      <c r="M77" t="str">
+        <v/>
+      </c>
+      <c r="N77" t="str">
+        <v/>
+      </c>
+      <c r="O77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C78" t="str">
+        <v/>
+      </c>
+      <c r="D78" t="str">
+        <v/>
+      </c>
+      <c r="E78" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F78" t="str">
+        <v/>
+      </c>
+      <c r="G78" t="str">
+        <v/>
+      </c>
+      <c r="H78" t="str">
+        <v>*</v>
+      </c>
+      <c r="I78" t="str">
+        <v>*</v>
+      </c>
+      <c r="J78" t="str">
+        <v>*</v>
+      </c>
+      <c r="K78" t="str">
+        <v/>
+      </c>
+      <c r="L78" t="str">
+        <v/>
+      </c>
+      <c r="M78" t="str">
+        <v/>
+      </c>
+      <c r="N78" t="str">
+        <v/>
+      </c>
+      <c r="O78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C79" t="str">
+        <v/>
+      </c>
+      <c r="D79" t="str">
+        <v/>
+      </c>
+      <c r="E79" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F79" t="str">
+        <v/>
+      </c>
+      <c r="G79" t="str">
+        <v/>
+      </c>
+      <c r="H79" t="str">
+        <v/>
+      </c>
+      <c r="I79" t="str">
+        <v>*</v>
+      </c>
+      <c r="J79" t="str">
+        <v/>
+      </c>
+      <c r="K79" t="str">
+        <v/>
+      </c>
+      <c r="L79" t="str">
+        <v/>
+      </c>
+      <c r="M79" t="str">
+        <v/>
+      </c>
+      <c r="N79" t="str">
+        <v/>
+      </c>
+      <c r="O79" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C82" t="str" cm="1">
+        <f t="array" ref="C82:G86">_xlfn.MAKEARRAY(5,5,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=2,_xlpm.r-1+_xlpm.c-1&gt;=2,_xlpm.r-1+_xlpm.c-1&lt;=6,_xlpm.r-1-_xlpm.c+1&gt;=-2),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D82" t="str">
+        <v/>
+      </c>
+      <c r="E82" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F82" t="str">
+        <v/>
+      </c>
+      <c r="G82" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C83" t="str">
+        <v/>
+      </c>
+      <c r="D83" t="str">
+        <v>*</v>
+      </c>
+      <c r="E83" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F83" t="str">
+        <v>*</v>
+      </c>
+      <c r="G83" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C84" t="str">
+        <v>*</v>
+      </c>
+      <c r="D84" t="str">
+        <v>*</v>
+      </c>
+      <c r="E84" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F84" t="str">
+        <v>*</v>
+      </c>
+      <c r="G84" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C85" t="str">
+        <v/>
+      </c>
+      <c r="D85" t="str">
+        <v>*</v>
+      </c>
+      <c r="E85" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F85" t="str">
+        <v>*</v>
+      </c>
+      <c r="G85" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C86" t="str">
+        <v/>
+      </c>
+      <c r="D86" t="str">
+        <v/>
+      </c>
+      <c r="E86" s="4" t="str">
+        <v>*</v>
+      </c>
+      <c r="F86" t="str">
+        <v/>
+      </c>
+      <c r="G86" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C88" t="str" cm="1">
+        <f t="array" ref="C88:E90">_xlfn.MAKEARRAY(3,3,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=1,_xlpm.r-1+_xlpm.c-1&gt;=1,_xlpm.r-1+_xlpm.c-1&lt;=3,_xlpm.r-1-_xlpm.c+1&gt;=-1),"*","")))</f>
+        <v/>
+      </c>
+      <c r="D88" t="str">
+        <v>*</v>
+      </c>
+      <c r="E88" s="4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C89" t="str">
+        <v>*</v>
+      </c>
+      <c r="D89" t="str">
+        <v>*</v>
+      </c>
+      <c r="E89" s="4" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C90" t="str">
+        <v/>
+      </c>
+      <c r="D90" t="str">
+        <v>*</v>
+      </c>
+      <c r="E90" s="4" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1577,8 +4179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36980439-0376-4A92-93D2-9D66C85EB6B6}">
   <dimension ref="C1:BD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="AG37" sqref="AG37"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="AX55" sqref="AX55:AX61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Created a generalized odd solution
</commit_message>
<xml_diff>
--- a/CH-77 Character-Based Rhombus.xlsx
+++ b/CH-77 Character-Based Rhombus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F555458-9AE7-4D79-AC29-55C60DD79544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D87D64E-9528-47A2-967E-8B08C36B403D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="2">
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>This solves the odd case. The even case will be similar and won't teach me anything new.</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B17870-5941-4C59-8CD8-DDAC51A6FF70}">
   <dimension ref="C1:AK90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="Y55" sqref="Y55"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="V65" sqref="V65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,7 +1137,7 @@
     <col min="5" max="5" width="2.44140625" style="4" customWidth="1"/>
     <col min="6" max="17" width="2.44140625" customWidth="1"/>
     <col min="18" max="19" width="2.77734375" customWidth="1"/>
-    <col min="23" max="23" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="32" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:37" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3515,9 +3518,22 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:32" x14ac:dyDescent="0.3">
+      <c r="V65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C67" t="str" cm="1">
-        <f t="array" ref="C67:O79">_xlfn.MAKEARRAY(13,13,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(AND(_xlpm.r-1-_xlpm.c+1&lt;=6,_xlpm.r-1+_xlpm.c-1&gt;=6,_xlpm.r-1+_xlpm.c-1&lt;=18,_xlpm.r-1-_xlpm.c+1&gt;=-6),"*","")))</f>
+        <f t="array" ref="C67:O79">_xlfn.MAKEARRAY(13,13,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,
+                        _xlfn.LET(_xlpm.rz,_xlpm.r-1,
+                            _xlpm.cz,_xlpm.c-1,
+                            IF(AND(_xlpm.rz-_xlpm.cz&lt;=6,_xlpm.rz+_xlpm.cz&gt;=6,_xlpm.rz+_xlpm.cz&lt;=18,_xlpm.rz-_xlpm.cz&gt;=-6),
+                               "*",""
+                              )
+                           )
+                       )
+           )</f>
         <v/>
       </c>
       <c r="D67" t="str">
@@ -3556,8 +3572,51 @@
       <c r="O67" t="str">
         <v/>
       </c>
-    </row>
-    <row r="68" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V67" t="str" cm="1">
+        <f t="array" ref="V67:AF77">_xlfn.LET(_xlpm.N,11,_xlfn.MAKEARRAY(_xlpm.N,_xlpm.N,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,
+                        _xlfn.LET(_xlpm.rz,_xlpm.r-1,
+                            _xlpm.cz,_xlpm.c-1,
+                            _xlpm.nz,INT(_xlpm.N/2),
+                            IF(AND(_xlpm.rz-_xlpm.cz&lt;=_xlpm.nz,_xlpm.rz+_xlpm.cz&gt;=_xlpm.nz,_xlpm.rz+_xlpm.cz&lt;=_xlpm.N*1.5-1.5,_xlpm.rz-_xlpm.cz&gt;=-_xlpm.nz),
+                               "*",""
+                              )
+                           )
+                       )
+           ))</f>
+        <v/>
+      </c>
+      <c r="W67" t="str">
+        <v/>
+      </c>
+      <c r="X67" t="str">
+        <v/>
+      </c>
+      <c r="Y67" t="str">
+        <v/>
+      </c>
+      <c r="Z67" t="str">
+        <v/>
+      </c>
+      <c r="AA67" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB67" t="str">
+        <v/>
+      </c>
+      <c r="AC67" t="str">
+        <v/>
+      </c>
+      <c r="AD67" t="str">
+        <v/>
+      </c>
+      <c r="AE67" t="str">
+        <v/>
+      </c>
+      <c r="AF67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C68" t="str">
         <v/>
       </c>
@@ -3597,8 +3656,41 @@
       <c r="O68" t="str">
         <v/>
       </c>
-    </row>
-    <row r="69" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V68" t="str">
+        <v/>
+      </c>
+      <c r="W68" t="str">
+        <v/>
+      </c>
+      <c r="X68" t="str">
+        <v/>
+      </c>
+      <c r="Y68" t="str">
+        <v/>
+      </c>
+      <c r="Z68" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA68" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB68" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC68" t="str">
+        <v/>
+      </c>
+      <c r="AD68" t="str">
+        <v/>
+      </c>
+      <c r="AE68" t="str">
+        <v/>
+      </c>
+      <c r="AF68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C69" t="str">
         <v/>
       </c>
@@ -3638,8 +3730,41 @@
       <c r="O69" t="str">
         <v/>
       </c>
-    </row>
-    <row r="70" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V69" t="str">
+        <v/>
+      </c>
+      <c r="W69" t="str">
+        <v/>
+      </c>
+      <c r="X69" t="str">
+        <v/>
+      </c>
+      <c r="Y69" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z69" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA69" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB69" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC69" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD69" t="str">
+        <v/>
+      </c>
+      <c r="AE69" t="str">
+        <v/>
+      </c>
+      <c r="AF69" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C70" t="str">
         <v/>
       </c>
@@ -3679,8 +3804,41 @@
       <c r="O70" t="str">
         <v/>
       </c>
-    </row>
-    <row r="71" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V70" t="str">
+        <v/>
+      </c>
+      <c r="W70" t="str">
+        <v/>
+      </c>
+      <c r="X70" t="str">
+        <v>*</v>
+      </c>
+      <c r="Y70" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z70" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA70" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB70" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC70" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD70" t="str">
+        <v>*</v>
+      </c>
+      <c r="AE70" t="str">
+        <v/>
+      </c>
+      <c r="AF70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C71" t="str">
         <v/>
       </c>
@@ -3720,8 +3878,41 @@
       <c r="O71" t="str">
         <v/>
       </c>
-    </row>
-    <row r="72" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V71" t="str">
+        <v/>
+      </c>
+      <c r="W71" t="str">
+        <v>*</v>
+      </c>
+      <c r="X71" t="str">
+        <v>*</v>
+      </c>
+      <c r="Y71" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z71" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA71" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB71" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC71" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD71" t="str">
+        <v>*</v>
+      </c>
+      <c r="AE71" t="str">
+        <v>*</v>
+      </c>
+      <c r="AF71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C72" t="str">
         <v/>
       </c>
@@ -3761,8 +3952,41 @@
       <c r="O72" t="str">
         <v/>
       </c>
-    </row>
-    <row r="73" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V72" t="str">
+        <v>*</v>
+      </c>
+      <c r="W72" t="str">
+        <v>*</v>
+      </c>
+      <c r="X72" t="str">
+        <v>*</v>
+      </c>
+      <c r="Y72" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z72" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA72" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB72" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC72" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD72" t="str">
+        <v>*</v>
+      </c>
+      <c r="AE72" t="str">
+        <v>*</v>
+      </c>
+      <c r="AF72" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="73" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C73" t="str">
         <v>*</v>
       </c>
@@ -3802,8 +4026,41 @@
       <c r="O73" t="str">
         <v>*</v>
       </c>
-    </row>
-    <row r="74" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V73" t="str">
+        <v/>
+      </c>
+      <c r="W73" t="str">
+        <v>*</v>
+      </c>
+      <c r="X73" t="str">
+        <v>*</v>
+      </c>
+      <c r="Y73" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z73" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA73" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB73" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC73" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD73" t="str">
+        <v>*</v>
+      </c>
+      <c r="AE73" t="str">
+        <v>*</v>
+      </c>
+      <c r="AF73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C74" t="str">
         <v/>
       </c>
@@ -3843,8 +4100,41 @@
       <c r="O74" t="str">
         <v/>
       </c>
-    </row>
-    <row r="75" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V74" t="str">
+        <v/>
+      </c>
+      <c r="W74" t="str">
+        <v/>
+      </c>
+      <c r="X74" t="str">
+        <v>*</v>
+      </c>
+      <c r="Y74" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z74" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA74" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB74" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC74" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD74" t="str">
+        <v>*</v>
+      </c>
+      <c r="AE74" t="str">
+        <v/>
+      </c>
+      <c r="AF74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C75" t="str">
         <v/>
       </c>
@@ -3884,8 +4174,41 @@
       <c r="O75" t="str">
         <v/>
       </c>
-    </row>
-    <row r="76" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V75" t="str">
+        <v/>
+      </c>
+      <c r="W75" t="str">
+        <v/>
+      </c>
+      <c r="X75" t="str">
+        <v/>
+      </c>
+      <c r="Y75" t="str">
+        <v>*</v>
+      </c>
+      <c r="Z75" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA75" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB75" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC75" t="str">
+        <v>*</v>
+      </c>
+      <c r="AD75" t="str">
+        <v/>
+      </c>
+      <c r="AE75" t="str">
+        <v/>
+      </c>
+      <c r="AF75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C76" t="str">
         <v/>
       </c>
@@ -3925,8 +4248,41 @@
       <c r="O76" t="str">
         <v/>
       </c>
-    </row>
-    <row r="77" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V76" t="str">
+        <v/>
+      </c>
+      <c r="W76" t="str">
+        <v/>
+      </c>
+      <c r="X76" t="str">
+        <v/>
+      </c>
+      <c r="Y76" t="str">
+        <v/>
+      </c>
+      <c r="Z76" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA76" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB76" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC76" t="str">
+        <v/>
+      </c>
+      <c r="AD76" t="str">
+        <v/>
+      </c>
+      <c r="AE76" t="str">
+        <v/>
+      </c>
+      <c r="AF76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C77" t="str">
         <v/>
       </c>
@@ -3966,8 +4322,41 @@
       <c r="O77" t="str">
         <v/>
       </c>
-    </row>
-    <row r="78" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="V77" t="str">
+        <v/>
+      </c>
+      <c r="W77" t="str">
+        <v/>
+      </c>
+      <c r="X77" t="str">
+        <v/>
+      </c>
+      <c r="Y77" t="str">
+        <v/>
+      </c>
+      <c r="Z77" t="str">
+        <v/>
+      </c>
+      <c r="AA77" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB77" t="str">
+        <v/>
+      </c>
+      <c r="AC77" t="str">
+        <v/>
+      </c>
+      <c r="AD77" t="str">
+        <v/>
+      </c>
+      <c r="AE77" t="str">
+        <v/>
+      </c>
+      <c r="AF77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C78" t="str">
         <v/>
       </c>
@@ -4008,7 +4397,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:32" x14ac:dyDescent="0.3">
       <c r="C79" t="str">
         <v/>
       </c>

</xml_diff>